<commit_message>
fixed fiscal years for microsoft, added chatbot prototype
</commit_message>
<xml_diff>
--- a/Key_Financials__10-K__last_3_FYs_.xlsx
+++ b/Key_Financials__10-K__last_3_FYs_.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1c6721748869b99e/Northwood/BSGX/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1c6721748869b99e/Northwood/BSGX/BCG_X_From_Forage_10k/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C58ED318-BFDE-4220-A61C-671826C2D2E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{C58ED318-BFDE-4220-A61C-671826C2D2E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3864AA0-4740-4AC0-8555-8B189B38A45D}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13335" xr2:uid="{8305E3AA-DF6A-4813-A8AB-E4C85DD813EC}"/>
+    <workbookView xWindow="10718" yWindow="0" windowWidth="10965" windowHeight="6652" xr2:uid="{8305E3AA-DF6A-4813-A8AB-E4C85DD813EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Key_Financials__10-K__last_3_FY" sheetId="1" r:id="rId1"/>
@@ -916,7 +916,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F5D8BE9-1DA5-46BC-9F78-D3B8638FFE23}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
@@ -951,25 +953,25 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="C2" s="1">
-        <v>45838</v>
+        <v>45473</v>
       </c>
       <c r="D2">
-        <v>281724</v>
+        <v>245122</v>
       </c>
       <c r="E2">
-        <v>101832</v>
+        <v>88136</v>
       </c>
       <c r="F2">
-        <v>619003</v>
+        <v>512163</v>
       </c>
       <c r="G2">
-        <v>275524</v>
+        <v>243686</v>
       </c>
       <c r="H2">
-        <v>140814</v>
+        <v>118548</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
@@ -977,25 +979,25 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C3" s="1">
-        <v>45473</v>
+        <v>45107</v>
       </c>
       <c r="D3">
-        <v>245122</v>
+        <v>211915</v>
       </c>
       <c r="E3">
-        <v>88136</v>
+        <v>72361</v>
       </c>
       <c r="F3">
-        <v>512163</v>
+        <v>411976</v>
       </c>
       <c r="G3">
-        <v>243686</v>
+        <v>205753</v>
       </c>
       <c r="H3">
-        <v>118548</v>
+        <v>87582</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
@@ -1003,25 +1005,25 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C4" s="1">
-        <v>45107</v>
+        <v>44742</v>
       </c>
       <c r="D4">
-        <v>211915</v>
+        <v>198270</v>
       </c>
       <c r="E4">
-        <v>72361</v>
+        <v>72738</v>
       </c>
       <c r="F4">
-        <v>411976</v>
+        <v>364840</v>
       </c>
       <c r="G4">
-        <v>205753</v>
+        <v>198298</v>
       </c>
       <c r="H4">
-        <v>87582</v>
+        <v>89035</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
@@ -1182,5 +1184,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>